<commit_message>
U5: lcd driver, bulk capacitor
</commit_message>
<xml_diff>
--- a/documents/cubit_gantt_chart.xlsx
+++ b/documents/cubit_gantt_chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCE7E5-FF21-4B3F-98F6-42FFDBF9C9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12191307-C387-4560-9DDD-D8B7099DBF1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
   <si>
     <t>Project Planner</t>
   </si>
@@ -315,19 +315,49 @@
     <t>Finalize battery</t>
   </si>
   <si>
-    <t>Finalize solar panel</t>
-  </si>
-  <si>
     <t>Study voltage regulator Ics</t>
   </si>
   <si>
-    <t>BON Power supply circuit</t>
-  </si>
-  <si>
-    <t>Power supply schematic</t>
-  </si>
-  <si>
     <t>February 7th</t>
+  </si>
+  <si>
+    <t>Finalize Solar Panel</t>
+  </si>
+  <si>
+    <t>Interface LCD Display with Blue Gecko</t>
+  </si>
+  <si>
+    <t>Altium Component Library List</t>
+  </si>
+  <si>
+    <t>To be completed next week</t>
+  </si>
+  <si>
+    <t>Finalize bulk capacitance</t>
+  </si>
+  <si>
+    <t>Schematic for power management</t>
+  </si>
+  <si>
+    <t>Schematic for sensor interfacing</t>
+  </si>
+  <si>
+    <t>Complete layout of the product</t>
+  </si>
+  <si>
+    <t>Demo IDE finalize</t>
+  </si>
+  <si>
+    <t>Final schematic integration</t>
+  </si>
+  <si>
+    <t>Interfacing IMU sensor with Blue  Gecko</t>
+  </si>
+  <si>
+    <t>February 14th</t>
+  </si>
+  <si>
+    <t>February 22nd</t>
   </si>
 </sst>
 </file>
@@ -645,7 +675,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -772,6 +802,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90"/>
     </xf>
@@ -791,7 +824,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -804,7 +837,7 @@
     <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -877,34 +910,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -916,75 +921,19 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
       <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+        <top style="thin">
+          <color theme="7"/>
+        </top>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1019,119 +968,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1156,261 +992,6 @@
         </top>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1596,9 +1177,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>15</xdr:col>
-          <xdr:colOff>180975</xdr:colOff>
+          <xdr:colOff>184150</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>257175</xdr:rowOff>
+          <xdr:rowOff>260350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1870,19 +1451,19 @@
   </sheetPr>
   <dimension ref="B1:DV41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
     <col min="2" max="2" width="34.9140625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="25" style="15" customWidth="1"/>
+    <col min="3" max="3" width="12.4140625" style="15" customWidth="1"/>
     <col min="4" max="6" width="7.08203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.08203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.4140625" style="1" customWidth="1"/>
     <col min="10" max="14" width="2.75" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.25" style="1" customWidth="1"/>
     <col min="16" max="18" width="2.75" style="1" bestFit="1" customWidth="1"/>
@@ -2053,39 +1634,39 @@
       <c r="T2" s="24"/>
       <c r="X2" s="24"/>
       <c r="AB2" s="23"/>
-      <c r="AP2" s="45" t="s">
+      <c r="AP2" s="46" t="s">
         <v>23</v>
       </c>
       <c r="AR2" s="23"/>
-      <c r="BD2" s="45" t="s">
+      <c r="BD2" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="BI2" s="42" t="s">
+      <c r="BI2" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="BK2" s="45" t="s">
+      <c r="BK2" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="BN2" s="42" t="s">
+      <c r="BN2" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="BR2" s="45" t="s">
+      <c r="BR2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="BY2" s="45" t="s">
+      <c r="BY2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="CA2" s="46" t="s">
+      <c r="CA2" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="CB2" s="46"/>
-      <c r="CC2" s="46"/>
+      <c r="CB2" s="47"/>
+      <c r="CC2" s="47"/>
       <c r="CD2" s="41"/>
-      <c r="CE2" s="46"/>
-      <c r="CH2" s="45" t="s">
+      <c r="CE2" s="47"/>
+      <c r="CH2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="CO2" s="45" t="s">
+      <c r="CO2" s="46" t="s">
         <v>42</v>
       </c>
       <c r="DA2" s="23"/>
@@ -2097,13 +1678,13 @@
       <c r="DH2" s="23"/>
       <c r="DI2" s="23"/>
       <c r="DJ2" s="23"/>
-      <c r="DK2" s="42" t="s">
+      <c r="DK2" s="43" t="s">
         <v>45</v>
       </c>
       <c r="DO2" s="27"/>
       <c r="DP2" s="27"/>
       <c r="DQ2" s="27"/>
-      <c r="DR2" s="43" t="s">
+      <c r="DR2" s="44" t="s">
         <v>17</v>
       </c>
       <c r="DS2" s="27"/>
@@ -2111,36 +1692,36 @@
       <c r="DU2" s="23"/>
     </row>
     <row r="3" spans="2:126" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="B3" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
       <c r="J3" s="24"/>
       <c r="M3" s="24"/>
       <c r="N3" s="24"/>
       <c r="T3" s="24"/>
       <c r="X3" s="24"/>
       <c r="AB3" s="23"/>
-      <c r="AP3" s="45"/>
+      <c r="AP3" s="46"/>
       <c r="AR3" s="23"/>
-      <c r="BD3" s="45"/>
-      <c r="BI3" s="42"/>
-      <c r="BK3" s="45"/>
-      <c r="BN3" s="42"/>
-      <c r="BR3" s="45"/>
-      <c r="BY3" s="45"/>
-      <c r="CA3" s="46"/>
-      <c r="CB3" s="46"/>
-      <c r="CC3" s="46"/>
+      <c r="BD3" s="46"/>
+      <c r="BI3" s="43"/>
+      <c r="BK3" s="46"/>
+      <c r="BN3" s="43"/>
+      <c r="BR3" s="46"/>
+      <c r="BY3" s="46"/>
+      <c r="CA3" s="47"/>
+      <c r="CB3" s="47"/>
+      <c r="CC3" s="47"/>
       <c r="CD3" s="41"/>
-      <c r="CE3" s="46"/>
-      <c r="CH3" s="45"/>
-      <c r="CO3" s="45"/>
+      <c r="CE3" s="47"/>
+      <c r="CH3" s="46"/>
+      <c r="CO3" s="46"/>
       <c r="DA3" s="23"/>
       <c r="DB3" s="23"/>
       <c r="DC3" s="23"/>
@@ -2150,23 +1731,23 @@
       <c r="DH3" s="23"/>
       <c r="DI3" s="23"/>
       <c r="DJ3" s="23"/>
-      <c r="DK3" s="42"/>
+      <c r="DK3" s="43"/>
       <c r="DO3" s="27"/>
       <c r="DP3" s="27"/>
       <c r="DQ3" s="27"/>
-      <c r="DR3" s="44"/>
+      <c r="DR3" s="45"/>
       <c r="DS3" s="27"/>
       <c r="DT3" s="23"/>
       <c r="DU3" s="23"/>
     </row>
     <row r="4" spans="2:126" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
       <c r="J4" s="5" t="s">
         <v>19</v>
       </c>
@@ -2198,21 +1779,21 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="24"/>
-      <c r="AP4" s="45"/>
+      <c r="AP4" s="46"/>
       <c r="AR4" s="23"/>
-      <c r="BD4" s="45"/>
-      <c r="BI4" s="42"/>
-      <c r="BK4" s="45"/>
-      <c r="BN4" s="42"/>
-      <c r="BR4" s="45"/>
-      <c r="BY4" s="45"/>
-      <c r="CA4" s="46"/>
-      <c r="CB4" s="46"/>
-      <c r="CC4" s="46"/>
+      <c r="BD4" s="46"/>
+      <c r="BI4" s="43"/>
+      <c r="BK4" s="46"/>
+      <c r="BN4" s="43"/>
+      <c r="BR4" s="46"/>
+      <c r="BY4" s="46"/>
+      <c r="CA4" s="47"/>
+      <c r="CB4" s="47"/>
+      <c r="CC4" s="47"/>
       <c r="CD4" s="41"/>
-      <c r="CE4" s="46"/>
-      <c r="CH4" s="45"/>
-      <c r="CO4" s="45"/>
+      <c r="CE4" s="47"/>
+      <c r="CH4" s="46"/>
+      <c r="CO4" s="46"/>
       <c r="DA4" s="23"/>
       <c r="DB4" s="23"/>
       <c r="DC4" s="23"/>
@@ -2222,23 +1803,23 @@
       <c r="DH4" s="23"/>
       <c r="DI4" s="23"/>
       <c r="DJ4" s="23"/>
-      <c r="DK4" s="42"/>
+      <c r="DK4" s="43"/>
       <c r="DO4" s="27"/>
       <c r="DP4" s="27"/>
       <c r="DQ4" s="27"/>
-      <c r="DR4" s="44"/>
+      <c r="DR4" s="45"/>
       <c r="DS4" s="27"/>
       <c r="DT4" s="23"/>
       <c r="DU4" s="23"/>
     </row>
     <row r="5" spans="2:126" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="J5" s="24"/>
       <c r="M5" s="24"/>
       <c r="N5" s="24"/>
@@ -2255,21 +1836,21 @@
       <c r="AB5"/>
       <c r="AC5"/>
       <c r="AG5" s="23"/>
-      <c r="AP5" s="45"/>
+      <c r="AP5" s="46"/>
       <c r="AR5" s="23"/>
-      <c r="BD5" s="45"/>
-      <c r="BI5" s="42"/>
-      <c r="BK5" s="45"/>
-      <c r="BN5" s="42"/>
-      <c r="BR5" s="45"/>
-      <c r="BY5" s="45"/>
-      <c r="CA5" s="46"/>
-      <c r="CB5" s="46"/>
-      <c r="CC5" s="46"/>
+      <c r="BD5" s="46"/>
+      <c r="BI5" s="43"/>
+      <c r="BK5" s="46"/>
+      <c r="BN5" s="43"/>
+      <c r="BR5" s="46"/>
+      <c r="BY5" s="46"/>
+      <c r="CA5" s="47"/>
+      <c r="CB5" s="47"/>
+      <c r="CC5" s="47"/>
       <c r="CD5" s="41"/>
-      <c r="CE5" s="46"/>
-      <c r="CH5" s="45"/>
-      <c r="CO5" s="45"/>
+      <c r="CE5" s="47"/>
+      <c r="CH5" s="46"/>
+      <c r="CO5" s="46"/>
       <c r="DA5" s="23"/>
       <c r="DB5" s="23"/>
       <c r="DC5" s="23"/>
@@ -2279,11 +1860,11 @@
       <c r="DH5" s="23"/>
       <c r="DI5" s="23"/>
       <c r="DJ5" s="23"/>
-      <c r="DK5" s="42"/>
+      <c r="DK5" s="43"/>
       <c r="DO5" s="27"/>
       <c r="DP5" s="27"/>
       <c r="DQ5" s="27"/>
-      <c r="DR5" s="44"/>
+      <c r="DR5" s="45"/>
       <c r="DS5" s="27"/>
       <c r="DT5" s="23"/>
       <c r="DU5" s="23"/>
@@ -2294,21 +1875,21 @@
       <c r="N6" s="24"/>
       <c r="T6" s="24"/>
       <c r="X6" s="24"/>
-      <c r="AP6" s="45"/>
+      <c r="AP6" s="46"/>
       <c r="AR6" s="23"/>
-      <c r="BD6" s="45"/>
-      <c r="BI6" s="42"/>
-      <c r="BK6" s="45"/>
-      <c r="BN6" s="42"/>
-      <c r="BR6" s="45"/>
-      <c r="BY6" s="45"/>
-      <c r="CA6" s="46"/>
-      <c r="CB6" s="46"/>
-      <c r="CC6" s="46"/>
+      <c r="BD6" s="46"/>
+      <c r="BI6" s="43"/>
+      <c r="BK6" s="46"/>
+      <c r="BN6" s="43"/>
+      <c r="BR6" s="46"/>
+      <c r="BY6" s="46"/>
+      <c r="CA6" s="47"/>
+      <c r="CB6" s="47"/>
+      <c r="CC6" s="47"/>
       <c r="CD6" s="41"/>
-      <c r="CE6" s="46"/>
-      <c r="CH6" s="45"/>
-      <c r="CO6" s="45"/>
+      <c r="CE6" s="47"/>
+      <c r="CH6" s="46"/>
+      <c r="CO6" s="46"/>
       <c r="DA6" s="23"/>
       <c r="DB6" s="23"/>
       <c r="DC6" s="23"/>
@@ -2318,11 +1899,11 @@
       <c r="DH6" s="23"/>
       <c r="DI6" s="23"/>
       <c r="DJ6" s="23"/>
-      <c r="DK6" s="42"/>
+      <c r="DK6" s="43"/>
       <c r="DO6" s="27"/>
       <c r="DP6" s="27"/>
       <c r="DQ6" s="27"/>
-      <c r="DR6" s="44"/>
+      <c r="DR6" s="45"/>
       <c r="DS6" s="27"/>
       <c r="DT6" s="23"/>
       <c r="DU6" s="23"/>
@@ -2352,11 +1933,11 @@
       <c r="K7" s="2"/>
       <c r="M7" s="31"/>
       <c r="N7" s="31"/>
-      <c r="P7" s="48" t="s">
+      <c r="P7" s="42" t="s">
         <v>62</v>
       </c>
       <c r="T7" s="29"/>
-      <c r="W7" s="48" t="s">
+      <c r="W7" s="42" t="s">
         <v>63</v>
       </c>
       <c r="X7" s="30"/>
@@ -2364,29 +1945,34 @@
         <v>46</v>
       </c>
       <c r="AK7" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP7" s="45"/>
-      <c r="AR7" s="31"/>
-      <c r="BD7" s="45"/>
+        <v>67</v>
+      </c>
+      <c r="AP7" s="46"/>
+      <c r="AR7" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ7" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="BD7" s="46"/>
       <c r="BG7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="BI7" s="42"/>
-      <c r="BK7" s="45"/>
-      <c r="BN7" s="42"/>
-      <c r="BR7" s="45"/>
-      <c r="BY7" s="45"/>
-      <c r="CA7" s="46"/>
-      <c r="CB7" s="46"/>
-      <c r="CC7" s="46"/>
+      <c r="BI7" s="43"/>
+      <c r="BK7" s="46"/>
+      <c r="BN7" s="43"/>
+      <c r="BR7" s="46"/>
+      <c r="BY7" s="46"/>
+      <c r="CA7" s="47"/>
+      <c r="CB7" s="47"/>
+      <c r="CC7" s="47"/>
       <c r="CD7" s="41"/>
-      <c r="CE7" s="46"/>
-      <c r="CH7" s="45"/>
+      <c r="CE7" s="47"/>
+      <c r="CH7" s="46"/>
       <c r="CL7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="CO7" s="45"/>
+      <c r="CO7" s="46"/>
       <c r="DA7" s="23"/>
       <c r="DB7" s="23"/>
       <c r="DC7" s="23"/>
@@ -2395,7 +1981,7 @@
       <c r="DH7" s="23"/>
       <c r="DI7" s="23"/>
       <c r="DJ7" s="23"/>
-      <c r="DK7" s="42"/>
+      <c r="DK7" s="43"/>
       <c r="DO7" s="28" t="s">
         <v>20</v>
       </c>
@@ -2403,7 +1989,7 @@
         <v>49</v>
       </c>
       <c r="DQ7" s="27"/>
-      <c r="DR7" s="44"/>
+      <c r="DR7" s="45"/>
       <c r="DS7" s="27"/>
       <c r="DT7" s="23"/>
       <c r="DU7" s="23"/>
@@ -2991,13 +2577,13 @@
         <v>59</v>
       </c>
       <c r="D12" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E12" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F12" s="12">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G12" s="12">
         <v>3</v>
@@ -3132,7 +2718,7 @@
         <v>65</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="12">
         <v>23</v>
@@ -3141,13 +2727,13 @@
         <v>3</v>
       </c>
       <c r="F18" s="12">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H18" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="20"/>
     </row>
@@ -3156,125 +2742,133 @@
         <v>66</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="12">
+        <v>22</v>
+      </c>
+      <c r="E19" s="12">
+        <v>4</v>
+      </c>
+      <c r="F19" s="12">
         <v>23</v>
       </c>
-      <c r="E19" s="12">
-        <v>3</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
       <c r="G19" s="12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="12">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E20" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F20" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G20" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="18" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" s="12">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E21" s="12">
         <v>3</v>
       </c>
       <c r="F21" s="12">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D22" s="12">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E22" s="12">
         <v>3</v>
       </c>
       <c r="F22" s="12">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G22" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="18"/>
-      <c r="C23" s="22"/>
+      <c r="B23" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="D23" s="12">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E23" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F23" s="12">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G23" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H23" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="20"/>
     </row>
     <row r="24" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="18"/>
-      <c r="C24" s="22"/>
+      <c r="B24" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="D24" s="12">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E24" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24" s="12">
         <v>0</v>
@@ -3285,16 +2879,22 @@
       <c r="H24" s="13">
         <v>0</v>
       </c>
-      <c r="I24" s="20"/>
+      <c r="I24" s="20" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="18"/>
-      <c r="C25" s="22"/>
+      <c r="B25" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>61</v>
+      </c>
       <c r="D25" s="12">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E25" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F25" s="12">
         <v>0</v>
@@ -3308,13 +2908,17 @@
       <c r="I25" s="20"/>
     </row>
     <row r="26" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="18"/>
-      <c r="C26" s="22"/>
+      <c r="B26" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>60</v>
+      </c>
       <c r="D26" s="12">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E26" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26" s="12">
         <v>0</v>
@@ -3328,13 +2932,17 @@
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="18"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="D27" s="12">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E27" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F27" s="12">
         <v>0</v>
@@ -3348,13 +2956,17 @@
       <c r="I27" s="20"/>
     </row>
     <row r="28" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="18"/>
-      <c r="C28" s="22"/>
+      <c r="B28" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="D28" s="12">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E28" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F28" s="12">
         <v>0</v>
@@ -3368,13 +2980,17 @@
       <c r="I28" s="20"/>
     </row>
     <row r="29" spans="2:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="18"/>
-      <c r="C29" s="22"/>
+      <c r="B29" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="22" t="s">
+        <v>59</v>
+      </c>
       <c r="D29" s="12">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="E29" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F29" s="12">
         <v>0</v>
@@ -3614,174 +3230,70 @@
     <mergeCell ref="CA2:CA7"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="J10:BQ41">
-    <cfRule type="expression" dxfId="51" priority="44">
+  <conditionalFormatting sqref="J10:DU41">
+    <cfRule type="expression" dxfId="19" priority="44">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="46">
+    <cfRule type="expression" dxfId="18" priority="46">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="47">
+    <cfRule type="expression" dxfId="17" priority="47">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="48">
+    <cfRule type="expression" dxfId="16" priority="48">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="49">
+    <cfRule type="expression" dxfId="15" priority="49">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="50">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>J$9=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="54">
+    <cfRule type="expression" dxfId="13" priority="54">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="55">
+    <cfRule type="expression" dxfId="12" priority="55">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42:BQ42">
-    <cfRule type="expression" dxfId="43" priority="45">
+    <cfRule type="expression" dxfId="11" priority="45">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BW9 DU9">
-    <cfRule type="expression" dxfId="42" priority="51">
+    <cfRule type="expression" dxfId="10" priority="51">
       <formula>J$9=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BR10:CI41">
-    <cfRule type="expression" dxfId="41" priority="34">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="36">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="37">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="38">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="39">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="40">
-      <formula>BR$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="42">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="43">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="BR42:CI42">
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="9" priority="35">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BX9:CI9">
-    <cfRule type="expression" dxfId="32" priority="41">
+    <cfRule type="expression" dxfId="8" priority="41">
       <formula>BX$9=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CJ10:DA41">
-    <cfRule type="expression" dxfId="31" priority="24">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>CJ$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="32">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="CJ42:DA42">
-    <cfRule type="expression" dxfId="23" priority="25">
+    <cfRule type="expression" dxfId="7" priority="25">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CJ9:CZ9">
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="6" priority="31">
       <formula>CJ$9=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="DB10:DC41">
-    <cfRule type="expression" dxfId="21" priority="14">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="17">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="18">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="19">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="20">
-      <formula>DB$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="22">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="23">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="DB42:DC42">
-    <cfRule type="expression" dxfId="13" priority="15">
+    <cfRule type="expression" dxfId="5" priority="15">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DB9:DC9">
-    <cfRule type="expression" dxfId="12" priority="21">
+    <cfRule type="expression" dxfId="4" priority="21">
       <formula>DB$9=period_selected</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="DD10:DU41">
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>DD$9=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="13">
-      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DD42:DU42">
@@ -3840,15 +3352,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <APDescription xmlns="4873beb7-5857-4685-be1f-d57550cc96cc">Use this project planner to track your project by unique activities using the Gantt chart model. Easily see where each activity is according to plan.</APDescription>
@@ -3974,7 +3477,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x0101006EDDDB5EE6D98C44930B742096920B300400F5B6D36B3EF94B4E9A635CDF2A18F5B8" ma:contentTypeVersion="72" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a23e56308344d904b51738559c3d67c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4873beb7-5857-4685-be1f-d57550cc96cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd0908cc4600e77bf5da051303e00c8d" ns2:_="">
     <xsd:import namespace="4873beb7-5857-4685-be1f-d57550cc96cc"/>
@@ -5014,15 +4517,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034D67AC-589E-4C00-9B1A-F2A41167CA08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8873101-05C7-48A9-9E2E-94984378E3B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -5038,7 +4542,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0602295-AD8B-4999-B800-E8C6FA359398}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5054,4 +4558,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{034D67AC-589E-4C00-9B1A-F2A41167CA08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>